<commit_message>
gathered all needed inputs from user
</commit_message>
<xml_diff>
--- a/output/BUDGETtest.xlsx
+++ b/output/BUDGETtest.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Condo" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="2022-11-test" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="2022-11" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2022-12" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2022-11" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
@@ -79,13 +80,13 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
+      <color indexed="8"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color indexed="8"/>
+      <b val="1"/>
       <sz val="12"/>
     </font>
     <font>
@@ -567,11 +568,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="20" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -588,7 +589,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -600,7 +601,119 @@
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
     <cellStyle name="header" xfId="2"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00CCFF"/>
+          <bgColor rgb="FF00CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEE1111"/>
+          <bgColor rgb="FFEE1111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00CCFF"/>
+          <bgColor rgb="FF00CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEE1111"/>
+          <bgColor rgb="FFEE1111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00CCFF"/>
+          <bgColor rgb="FF00CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEE1111"/>
+          <bgColor rgb="FFEE1111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00CCFF"/>
+          <bgColor rgb="FF00CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEE1111"/>
+          <bgColor rgb="FFEE1111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00CCFF"/>
+          <bgColor rgb="FF00CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEE1111"/>
+          <bgColor rgb="FFEE1111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00CCFF"/>
+          <bgColor rgb="FF00CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEE1111"/>
+          <bgColor rgb="FFEE1111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00CCFF"/>
+          <bgColor rgb="FF00CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEE1111"/>
+          <bgColor rgb="FFEE1111"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2422,8 +2535,8 @@
     <col width="34.33203125" customWidth="1" style="38" min="6" max="6"/>
     <col width="8.1640625" customWidth="1" style="38" min="7" max="7"/>
     <col width="25.1640625" customWidth="1" style="38" min="8" max="11"/>
-    <col width="8.33203125" customWidth="1" style="38" min="12" max="53"/>
-    <col width="8.33203125" customWidth="1" style="38" min="54" max="16384"/>
+    <col width="8.33203125" customWidth="1" style="38" min="12" max="54"/>
+    <col width="8.33203125" customWidth="1" style="38" min="55" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.5" customHeight="1">
@@ -4148,7 +4261,1261 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" outlineLevelCol="0"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="44.33203125" customWidth="1" min="2" max="2"/>
+    <col width="19.6640625" customWidth="1" min="3" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+    <col width="46.6640625" customWidth="1" min="6" max="6"/>
+    <col width="24.6640625" customWidth="1" min="7" max="7"/>
+    <col width="8.6640625" customWidth="1" min="8" max="8"/>
+    <col width="5" customWidth="1" min="9" max="9"/>
+    <col width="11" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="29" t="inlineStr">
+        <is>
+          <t>Account Type</t>
+        </is>
+      </c>
+      <c r="C1" s="29" t="inlineStr">
+        <is>
+          <t>Account Number</t>
+        </is>
+      </c>
+      <c r="D1" s="29" t="inlineStr">
+        <is>
+          <t>Transaction Date</t>
+        </is>
+      </c>
+      <c r="E1" s="29" t="inlineStr">
+        <is>
+          <t>Cheque Number</t>
+        </is>
+      </c>
+      <c r="F1" s="29" t="inlineStr">
+        <is>
+          <t>Description 1</t>
+        </is>
+      </c>
+      <c r="G1" s="29" t="inlineStr">
+        <is>
+          <t>Description 2</t>
+        </is>
+      </c>
+      <c r="H1" s="29" t="inlineStr">
+        <is>
+          <t>CAD$</t>
+        </is>
+      </c>
+      <c r="I1" s="29" t="inlineStr">
+        <is>
+          <t>USD$</t>
+        </is>
+      </c>
+      <c r="J1" s="29" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="29" t="n">
+        <v>101</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Chequing</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>09231-5038385</t>
+        </is>
+      </c>
+      <c r="D2" s="27" t="n">
+        <v>44896</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>LOAN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RBC LOAN PYMT </t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>-119.32</v>
+      </c>
+      <c r="J2" s="28" t="inlineStr">
+        <is>
+          <t>loan</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="29" t="n">
+        <v>107</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chequing</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>09231-5038385</t>
+        </is>
+      </c>
+      <c r="D3" s="27" t="n">
+        <v>44911</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>WWW TRF DDA - 2295</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="29" t="n">
+        <v>108</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Chequing</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>09231-5038385</t>
+        </is>
+      </c>
+      <c r="D4" s="27" t="n">
+        <v>44911</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Transfer</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WWW TRANSFER - 1009 </t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="29" t="n">
+        <v>109</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Chequing</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>09231-5038385</t>
+        </is>
+      </c>
+      <c r="D5" s="27" t="n">
+        <v>44911</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Transfer</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WWW TRANSFER - 2214 </t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>-650</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="29" t="n">
+        <v>111</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Chequing</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>09231-5038385</t>
+        </is>
+      </c>
+      <c r="D6" s="27" t="n">
+        <v>44914</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>WWW PAYMENT - N9648</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>-113.83</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="29" t="n">
+        <v>153</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Savings</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>09231-5146493</t>
+        </is>
+      </c>
+      <c r="D7" s="27" t="n">
+        <v>44914</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>WWW TRF DDA - 5398</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>-220</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="29" t="n">
+        <v>173</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D8" s="27" t="n">
+        <v>44897</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>LULULEMONCOM* 877-263-9300 BC</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>-89.68000000000001</v>
+      </c>
+      <c r="J8" s="28" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="29" t="n">
+        <v>174</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D9" s="27" t="n">
+        <v>44898</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>PHARMAPRIX #1912 MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>-17.05</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="29" t="n">
+        <v>175</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D10" s="27" t="n">
+        <v>44898</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>METRO ETS 2416 MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>-21.93</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="29" t="n">
+        <v>176</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D11" s="27" t="n">
+        <v>44898</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MCDONALD'S #40371 MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>-4.82</v>
+      </c>
+      <c r="J11" s="28" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="29" t="n">
+        <v>177</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D12" s="27" t="n">
+        <v>44898</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>AIRBNB * HMZJN8ZPQZ AIRBNB.COM</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>-218.08</v>
+      </c>
+      <c r="J12" s="39" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="29" t="n">
+        <v>178</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D13" s="27" t="n">
+        <v>44900</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>LULULEMONCOM* 877-263-9300 BC</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>-158.67</v>
+      </c>
+      <c r="J13" s="39" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="29" t="n">
+        <v>179</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D14" s="27" t="n">
+        <v>44901</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ADONIS GRIFFINTOWN MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>-19.84</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="29" t="n">
+        <v>180</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D15" s="27" t="n">
+        <v>44902</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>L'OEUFRIER CHABANEL MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>-22.41</v>
+      </c>
+      <c r="J15" s="28" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="29" t="n">
+        <v>181</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D16" s="27" t="n">
+        <v>44905</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>STM COTE VERTU DAN104 MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>-31.5</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="29" t="n">
+        <v>182</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D17" s="27" t="n">
+        <v>44905</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>IGA EXTRA VALLEE LACHINE QC</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>-25.27</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="29" t="n">
+        <v>183</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D18" s="27" t="n">
+        <v>44906</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>MEGAPLEX SPHERETECQPS SAINT LAURENTQC</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>-13.5</v>
+      </c>
+      <c r="J18" s="28" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="29" t="n">
+        <v>184</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D19" s="27" t="n">
+        <v>44906</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>DECATHLON MONTREAL EATON MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>-8.050000000000001</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="29" t="n">
+        <v>185</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D20" s="27" t="n">
+        <v>44906</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>DOLLARAMA # 314 MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>-1.15</v>
+      </c>
+      <c r="J20" s="28" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="29" t="n">
+        <v>186</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D21" s="27" t="n">
+        <v>44906</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>PHARMAPRIX #1825 MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>-4.01</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="29" t="n">
+        <v>187</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D22" s="27" t="n">
+        <v>44906</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>SEPHORA STE CATHERINE MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>-73.58</v>
+      </c>
+      <c r="J22" s="28" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="29" t="n">
+        <v>188</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D23" s="27" t="n">
+        <v>44908</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>STAPLESPRINT.CA RICHMOND HILLON</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>-5.74</v>
+      </c>
+      <c r="J23" s="28" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="29" t="n">
+        <v>189</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D24" s="27" t="n">
+        <v>44909</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>ADONIS GRIFFINTOWN MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>-15.18</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="29" t="n">
+        <v>190</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D25" s="27" t="n">
+        <v>44909</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>ROCH LE COQ MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>-13.53</v>
+      </c>
+      <c r="J25" s="28" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="29" t="n">
+        <v>191</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D26" s="27" t="n">
+        <v>44910</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>TIM HORTONS #7285 MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>-4.99</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="29" t="n">
+        <v>192</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D27" s="27" t="n">
+        <v>44910</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>McDonalds 40371 MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>-10.57</v>
+      </c>
+      <c r="J27" s="28" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="29" t="n">
+        <v>194</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D28" s="27" t="n">
+        <v>44911</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>VUA SANDWICHES MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>-7.18</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="29" t="n">
+        <v>195</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D29" s="27" t="n">
+        <v>44913</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>CSH SAINT-JOSEPH QUEBEC CITY QC</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>-7.07</v>
+      </c>
+      <c r="J29" s="28" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="29" t="n">
+        <v>196</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Visa</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>4514098511036571</t>
+        </is>
+      </c>
+      <c r="D30" s="27" t="n">
+        <v>44913</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>CHEZ ASHTON CENTRE VIL QUEBEC QC</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>-9.6</v>
+      </c>
+      <c r="J30" s="28" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="29" t="n">
+        <v>201</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MasterCard</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>5415903604805039</t>
+        </is>
+      </c>
+      <c r="D31" s="27" t="n">
+        <v>44898</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>AMZN Mktp CA*4D6H98JO3 WWW.AMAZON.CAON</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>-27.58</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="29" t="n">
+        <v>202</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MasterCard</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>5415903604805039</t>
+        </is>
+      </c>
+      <c r="D32" s="27" t="n">
+        <v>44903</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>APPLE.COM/BILL 866-712-7753 ON</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>-4.59</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="29" t="n">
+        <v>203</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>MasterCard</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>5415903604805039</t>
+        </is>
+      </c>
+      <c r="D33" s="27" t="n">
+        <v>44907</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>AMZN Mktp CA*EE5PL7RD3 WWW.AMAZON.CAON</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>-48.59</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="29" t="n">
+        <v>204</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MasterCard</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>5415903604805039</t>
+        </is>
+      </c>
+      <c r="D34" s="27" t="n">
+        <v>44909</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>AMZN Mktp CA*XE6U87G73 WWW.AMAZON.CAON</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>-56.43</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="29" t="n">
+        <v>206</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MasterCard</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>5415903604805039</t>
+        </is>
+      </c>
+      <c r="D35" s="27" t="n">
+        <v>44911</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>HTTPS://POUBELLEDUSKI. MONTREAL QC</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>-287.44</v>
+      </c>
+      <c r="J35" s="28" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="30" t="inlineStr">
+        <is>
+          <t>TRANSPORT</t>
+        </is>
+      </c>
+      <c r="B38">
+        <f>-1*SUMIF(J2:J35,"transport",H2:H35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="30" t="inlineStr">
+        <is>
+          <t>PHONE</t>
+        </is>
+      </c>
+      <c r="B39">
+        <f>-1*SUMIF(J2:J35,"phone",H2:H35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="30" t="inlineStr">
+        <is>
+          <t>SHOPPING</t>
+        </is>
+      </c>
+      <c r="B40">
+        <f>-1*SUMIF(J2:J35,"shopping",H2:H35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="30" t="inlineStr">
+        <is>
+          <t>ACTIVITY</t>
+        </is>
+      </c>
+      <c r="B41">
+        <f>-1*SUMIF(J2:J35,"activity",H2:H35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="30" t="inlineStr">
+        <is>
+          <t>FOOD</t>
+        </is>
+      </c>
+      <c r="B42">
+        <f>-1*SUMIF(J2:J35,"food",H2:H35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="30" t="inlineStr">
+        <is>
+          <t>GROCERY</t>
+        </is>
+      </c>
+      <c r="B43">
+        <f>-1*SUMIF(J2:J35,"grocery",H2:H35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="30" t="inlineStr">
+        <is>
+          <t>MOM</t>
+        </is>
+      </c>
+      <c r="B44">
+        <f>-1*SUMIF(J2:J35,"mom",H2:H35)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="cellIs" priority="1" operator="greaterThan" dxfId="1">
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="0">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
+    <cfRule type="cellIs" priority="3" operator="greaterThan" dxfId="1">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="lessThan" dxfId="0">
+      <formula>80</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" priority="5" operator="greaterThan" dxfId="1">
+      <formula>300</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="lessThan" dxfId="0">
+      <formula>300</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="cellIs" priority="7" operator="greaterThan" dxfId="1">
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="8" operator="lessThan" dxfId="0">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="cellIs" priority="9" operator="greaterThan" dxfId="1">
+      <formula>300</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="10" operator="lessThan" dxfId="0">
+      <formula>300</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
+    <cfRule type="cellIs" priority="11" operator="greaterThan" dxfId="1">
+      <formula>500</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="12" operator="lessThan" dxfId="0">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="cellIs" priority="13" operator="greaterThan" dxfId="1">
+      <formula>150</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="14" operator="lessThan" dxfId="0">
+      <formula>150</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4161,7 +5528,7 @@
     <col width="19.68" customWidth="1" min="3" max="3"/>
     <col width="19.68" customWidth="1" min="4" max="4"/>
     <col width="15.99" customWidth="1" min="5" max="5"/>
-    <col width="46.74" customWidth="1" min="6" max="6"/>
+    <col width="44.28" customWidth="1" min="6" max="6"/>
     <col width="24.6" customWidth="1" min="7" max="7"/>
     <col width="8.609999999999999" customWidth="1" min="8" max="8"/>
     <col width="4.92" customWidth="1" min="9" max="9"/>
@@ -4507,139 +5874,135 @@
     </row>
     <row r="11">
       <c r="A11" s="40" t="n">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Savings</t>
+          <t>Chequing</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>09231-5146493</t>
+          <t>09231-5038385</t>
         </is>
       </c>
       <c r="D11" s="41" t="n">
-        <v>44868</v>
+        <v>44895</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>WWW TRF DDA - 7539</t>
+          <t>WWW PAYMENT - N0552</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
-        <v>-350</v>
+        <v>-1500</v>
       </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="40" t="n">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Chequing</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4514098511036571</t>
+          <t>09231-5038385</t>
         </is>
       </c>
       <c r="D12" s="41" t="n">
-        <v>44866</v>
+        <v>44895</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>BILLETTERIE GARE LUCIEN LMONTREAL QC</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
+          <t>Transfer</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WWW TRANSFER - 8263 </t>
+        </is>
+      </c>
       <c r="H12" t="n">
-        <v>-37.5</v>
+        <v>-91.62</v>
       </c>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>transport</t>
-        </is>
-      </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="40" t="n">
-        <v>158</v>
+        <v>99</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Chequing</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4514098511036571</t>
+          <t>09231-5038385</t>
         </is>
       </c>
       <c r="D13" s="41" t="n">
-        <v>44867</v>
+        <v>44895</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Subway 27443 MontrEal QC</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
+          <t>Transfer</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WWW TRANSFER - 0044 </t>
+        </is>
+      </c>
       <c r="H13" t="n">
-        <v>-12.64</v>
+        <v>-400</v>
       </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>food</t>
-        </is>
-      </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="40" t="n">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>Savings</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4514098511036571</t>
+          <t>09231-5146493</t>
         </is>
       </c>
       <c r="D14" s="41" t="n">
-        <v>44867</v>
+        <v>44868</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>#530 SPORTS EXPERTS MONTREAL QC</t>
+          <t>WWW TRF DDA - 7539</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>-257.53</v>
+        <v>-350</v>
       </c>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>shopping</t>
-        </is>
-      </c>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="40" t="n">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -4652,24 +6015,24 @@
         </is>
       </c>
       <c r="D15" s="41" t="n">
-        <v>44870</v>
+        <v>44877</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>TOUR DE JEUX MONTREAL QC</t>
+          <t>MON AMI MONTREAL QC</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>-17.24</v>
+        <v>-200.91</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="40" t="n">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -4682,24 +6045,28 @@
         </is>
       </c>
       <c r="D16" s="41" t="n">
-        <v>44870</v>
+        <v>44878</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>MR. PRETZELS MONTREAL QC</t>
+          <t>STM LOGE CADILLAC N101 MONTREAL QC</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
-        <v>-4.93</v>
+        <v>-37.5</v>
       </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="40" t="n">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -4712,28 +6079,28 @@
         </is>
       </c>
       <c r="D17" s="41" t="n">
-        <v>44870</v>
+        <v>44878</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>CAFE MYRIADE MONTREAL QC</t>
+          <t>GARE PINE BEACH DORVAL QC</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>-4.9</v>
+        <v>-3.5</v>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t>food</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="40" t="n">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -4746,28 +6113,28 @@
         </is>
       </c>
       <c r="D18" s="41" t="n">
-        <v>44870</v>
+        <v>44884</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>METRO ETS 2416 MONTREAL QC</t>
+          <t>TIM HORTONS #7285 MONTREAL QC</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
-        <v>-19.44</v>
+        <v>-9.960000000000001</v>
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>food</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="40" t="n">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -4780,28 +6147,28 @@
         </is>
       </c>
       <c r="D19" s="41" t="n">
-        <v>44871</v>
+        <v>44884</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>STARBUCKS 800-782-7282 800-782-7282 ON</t>
+          <t>UBER CANADA/UBERTRIP TORONTO ON</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
-        <v>-25</v>
+        <v>-17.7</v>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>food</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="40" t="n">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -4814,24 +6181,28 @@
         </is>
       </c>
       <c r="D20" s="41" t="n">
-        <v>44871</v>
+        <v>44884</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>VILLE DE DORVAL AMENAG DORVAL QC</t>
+          <t>ADONIS GRIFFINTOWN MONTREAL QC</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
-        <v>-15.5</v>
+        <v>-10.36</v>
       </c>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="40" t="n">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -4844,24 +6215,28 @@
         </is>
       </c>
       <c r="D21" s="41" t="n">
-        <v>44874</v>
+        <v>44884</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>GLAMSTAR LIMITED 4029357733</t>
+          <t>ADONIS GRIFFINTOWN MONTREAL QC</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>-73.72</v>
+        <v>-3.45</v>
       </c>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="40" t="n">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -4874,17 +6249,17 @@
         </is>
       </c>
       <c r="D22" s="41" t="n">
-        <v>44874</v>
+        <v>44884</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>TIM HORTONS #7285 514-347-8521 QC</t>
+          <t>PRESOTEA GRIFFINTOWN MONTREAL QC</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
-        <v>-4.82</v>
+        <v>-9.19</v>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
@@ -4895,7 +6270,7 @@
     </row>
     <row r="23">
       <c r="A23" s="40" t="n">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -4908,28 +6283,28 @@
         </is>
       </c>
       <c r="D23" s="41" t="n">
-        <v>44874</v>
+        <v>44885</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>GARE CHABANEL MONTREAL QC</t>
+          <t>DECATHLON MONTREAL EATON MONTREAL QC</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
-        <v>-31.5</v>
+        <v>-18.4</v>
       </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>shopping</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="40" t="n">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -4942,24 +6317,28 @@
         </is>
       </c>
       <c r="D24" s="41" t="n">
-        <v>44877</v>
+        <v>44886</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>MON AMI MONTREAL QC</t>
+          <t>TIM HORTONS #7285 MONTREAL QC</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>-200.91</v>
+        <v>-3.43</v>
       </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="40" t="n">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -4972,28 +6351,28 @@
         </is>
       </c>
       <c r="D25" s="41" t="n">
-        <v>44878</v>
+        <v>44888</v>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>GARE PINE BEACH DORVAL QC</t>
+          <t>TIM HORTONS #7285 514-347-8521 QC</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>-3.5</v>
+        <v>-5.05</v>
       </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>food</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="40" t="n">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -5006,28 +6385,28 @@
         </is>
       </c>
       <c r="D26" s="41" t="n">
-        <v>44878</v>
+        <v>44891</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>STM LOGE CADILLAC N101 MONTREAL QC</t>
+          <t>PHARMAPRIX #0012 DORVAL QC</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>-37.5</v>
+        <v>-17.51</v>
       </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>shopping</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="40" t="n">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -5040,28 +6419,28 @@
         </is>
       </c>
       <c r="D27" s="41" t="n">
-        <v>44884</v>
+        <v>44891</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>UBER CANADA/UBERTRIP TORONTO ON</t>
+          <t>IGA #8247 DORVAL QC</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="n">
-        <v>-17.7</v>
+        <v>-54.97</v>
       </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="40" t="n">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -5074,28 +6453,24 @@
         </is>
       </c>
       <c r="D28" s="41" t="n">
-        <v>44884</v>
+        <v>44892</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>ADONIS GRIFFINTOWN MONTREAL QC</t>
+          <t>CHOCOLAT PRIVILEGE ATW MONTREAL QC</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>-10.36</v>
+        <v>-11.53</v>
       </c>
       <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>grocery</t>
-        </is>
-      </c>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="40" t="n">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -5108,28 +6483,28 @@
         </is>
       </c>
       <c r="D29" s="41" t="n">
-        <v>44884</v>
+        <v>44892</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>ADONIS GRIFFINTOWN MONTREAL QC</t>
+          <t>GARE PINE BEACH DORVAL QC</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
-        <v>-3.45</v>
+        <v>-31.5</v>
       </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="40" t="n">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -5142,28 +6517,24 @@
         </is>
       </c>
       <c r="D30" s="41" t="n">
-        <v>44884</v>
+        <v>44894</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>PRESOTEA GRIFFINTOWN MONTREAL QC</t>
+          <t>SSENSE MONTREAL QC</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
-        <v>-9.19</v>
+        <v>-77.03</v>
       </c>
       <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>food</t>
-        </is>
-      </c>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="40" t="n">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -5176,51 +6547,47 @@
         </is>
       </c>
       <c r="D31" s="41" t="n">
-        <v>44884</v>
+        <v>44895</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>TIM HORTONS #7285 MONTREAL QC</t>
+          <t>LULULEMONCOM* 877-263-9300 BC</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>-9.960000000000001</v>
+        <v>-67.84</v>
       </c>
       <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>food</t>
-        </is>
-      </c>
+      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="40" t="n">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>MasterCard</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>4514098511036571</t>
+          <t>5415903604805039</t>
         </is>
       </c>
       <c r="D32" s="41" t="n">
-        <v>44885</v>
+        <v>44881</v>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>DECATHLON MONTREAL EATON MONTREAL QC</t>
+          <t>Amazon.ca*HI5I780C0 AMAZON.CA ON</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
-        <v>-18.4</v>
+        <v>-7.81</v>
       </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
@@ -5231,50 +6598,50 @@
     </row>
     <row r="33">
       <c r="A33" s="40" t="n">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>MasterCard</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>4514098511036571</t>
+          <t>5415903604805039</t>
         </is>
       </c>
       <c r="D33" s="41" t="n">
-        <v>44886</v>
+        <v>44883</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>TIM HORTONS #7285 MONTREAL QC</t>
+          <t>Amazon.ca*HI9VQ4MG1 AMAZON.CA ON</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
-        <v>-3.43</v>
+        <v>-7.34</v>
       </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
-          <t>food</t>
+          <t>shopping</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="40" t="n">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Visa</t>
+          <t>MasterCard</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>4514098511036571</t>
+          <t>5415903604805039</t>
         </is>
       </c>
       <c r="D34" s="41" t="n">
@@ -5283,519 +6650,153 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>TIM HORTONS #7285 514-347-8521 QC</t>
+          <t>TELUS MOBILITY PREAUTH CALGARY AB</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
-        <v>-5.05</v>
+        <v>-76.47</v>
       </c>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
-          <t>food</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="40" t="n">
-        <v>182</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Visa</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>4514098511036571</t>
-        </is>
-      </c>
-      <c r="D35" s="41" t="n">
-        <v>44891</v>
-      </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>PHARMAPRIX #0012 DORVAL QC</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="n">
-        <v>-17.51</v>
-      </c>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>shopping</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="40" t="n">
-        <v>183</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Visa</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>4514098511036571</t>
-        </is>
-      </c>
-      <c r="D36" s="41" t="n">
-        <v>44891</v>
-      </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>IGA #8247 DORVAL QC</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="n">
-        <v>-54.97</v>
-      </c>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>grocery</t>
-        </is>
-      </c>
-    </row>
+          <t>phone</t>
+        </is>
+      </c>
+    </row>
+    <row r="35"/>
+    <row r="36"/>
     <row r="37">
-      <c r="A37" s="40" t="n">
-        <v>184</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Visa</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>4514098511036571</t>
-        </is>
-      </c>
-      <c r="D37" s="41" t="n">
-        <v>44892</v>
-      </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>CHOCOLAT PRIVILEGE ATW MONTREAL QC</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="n">
-        <v>-11.53</v>
-      </c>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
+      <c r="A37" s="42" t="inlineStr">
+        <is>
+          <t>TRANSPORT</t>
+        </is>
+      </c>
+      <c r="B37">
+        <f>-1*SUMIF(J2:J34,"transport",H2:H34)</f>
+        <v/>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="40" t="n">
-        <v>185</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Visa</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>4514098511036571</t>
-        </is>
-      </c>
-      <c r="D38" s="41" t="n">
-        <v>44892</v>
-      </c>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>GARE PINE BEACH DORVAL QC</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="n">
-        <v>-31.5</v>
-      </c>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>transport</t>
-        </is>
+      <c r="A38" s="42" t="inlineStr">
+        <is>
+          <t>PHONE</t>
+        </is>
+      </c>
+      <c r="B38">
+        <f>-1*SUMIF(J2:J34,"phone",H2:H34)</f>
+        <v/>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="40" t="n">
-        <v>191</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>MasterCard</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>5415903604805039</t>
-        </is>
-      </c>
-      <c r="D39" s="41" t="n">
-        <v>44868</v>
-      </c>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>APPLE.COM/BILL 866-712-7753 ON</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="n">
-        <v>-16.09</v>
-      </c>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>shopping</t>
-        </is>
+      <c r="A39" s="42" t="inlineStr">
+        <is>
+          <t>SHOPPING</t>
+        </is>
+      </c>
+      <c r="B39">
+        <f>-1*SUMIF(J2:J34,"shopping",H2:H34)</f>
+        <v/>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="40" t="n">
-        <v>192</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>MasterCard</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>5415903604805039</t>
-        </is>
-      </c>
-      <c r="D40" s="41" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>OTT* NAUGHTYGIRLFITNES SANTA CLARA CA</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="n">
-        <v>-13.86</v>
-      </c>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
+      <c r="A40" s="42" t="inlineStr">
+        <is>
+          <t>ACTIVITY</t>
+        </is>
+      </c>
+      <c r="B40">
+        <f>-1*SUMIF(J2:J34,"activity",H2:H34)</f>
+        <v/>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="40" t="n">
-        <v>193</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>MasterCard</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>5415903604805039</t>
-        </is>
-      </c>
-      <c r="D41" s="41" t="n">
-        <v>44874</v>
-      </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>BIXI MONTREAL MONTREAL QC</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="n">
-        <v>-20.7</v>
-      </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>transport</t>
-        </is>
+      <c r="A41" s="42" t="inlineStr">
+        <is>
+          <t>FOOD</t>
+        </is>
+      </c>
+      <c r="B41">
+        <f>-1*SUMIF(J2:J34,"food",H2:H34)</f>
+        <v/>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="40" t="n">
-        <v>194</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>MasterCard</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>5415903604805039</t>
-        </is>
-      </c>
-      <c r="D42" s="41" t="n">
-        <v>44875</v>
-      </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>APPLE.COM/BILL 866-712-7753 ON</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="n">
-        <v>-4.59</v>
-      </c>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>shopping</t>
-        </is>
+      <c r="A42" s="42" t="inlineStr">
+        <is>
+          <t>GROCERY</t>
+        </is>
+      </c>
+      <c r="B42">
+        <f>-1*SUMIF(J2:J34,"grocery",H2:H34)</f>
+        <v/>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="40" t="n">
-        <v>196</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>MasterCard</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>5415903604805039</t>
-        </is>
-      </c>
-      <c r="D43" s="41" t="n">
-        <v>44881</v>
-      </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Amazon.ca*HI5I780C0 AMAZON.CA ON</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="n">
-        <v>-7.81</v>
-      </c>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>shopping</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="40" t="n">
-        <v>197</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>MasterCard</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>5415903604805039</t>
-        </is>
-      </c>
-      <c r="D44" s="41" t="n">
-        <v>44883</v>
-      </c>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Amazon.ca*HI9VQ4MG1 AMAZON.CA ON</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="n">
-        <v>-7.34</v>
-      </c>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>shopping</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="40" t="n">
-        <v>198</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>MasterCard</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>5415903604805039</t>
-        </is>
-      </c>
-      <c r="D45" s="41" t="n">
-        <v>44888</v>
-      </c>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>TELUS MOBILITY PREAUTH CALGARY AB</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="n">
-        <v>-76.47</v>
-      </c>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>phone</t>
-        </is>
-      </c>
-    </row>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48">
-      <c r="A48" s="42" t="inlineStr">
-        <is>
-          <t>TRANSPORT</t>
-        </is>
-      </c>
-      <c r="B48">
-        <f>-1*SUMIF(J2:J45,"transport",H2:H45)</f>
+      <c r="A43" s="42" t="inlineStr">
+        <is>
+          <t>MOM</t>
+        </is>
+      </c>
+      <c r="B43">
+        <f>-1*SUMIF(J2:J34,"mom",H2:H34)</f>
         <v/>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="42" t="inlineStr">
-        <is>
-          <t>PHONE</t>
-        </is>
-      </c>
-      <c r="B49">
-        <f>-1*SUMIF(J2:J45,"phone",H2:H45)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="42" t="inlineStr">
-        <is>
-          <t>SHOPPING</t>
-        </is>
-      </c>
-      <c r="B50">
-        <f>-1*SUMIF(J2:J45,"shopping",H2:H45)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="42" t="inlineStr">
-        <is>
-          <t>ACTIVITY</t>
-        </is>
-      </c>
-      <c r="B51">
-        <f>-1*SUMIF(J2:J45,"activity",H2:H45)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="42" t="inlineStr">
-        <is>
-          <t>FOOD</t>
-        </is>
-      </c>
-      <c r="B52">
-        <f>-1*SUMIF(J2:J45,"food",H2:H45)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="42" t="inlineStr">
-        <is>
-          <t>GROCERY</t>
-        </is>
-      </c>
-      <c r="B53">
-        <f>-1*SUMIF(J2:J45,"grocery",H2:H45)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="42" t="inlineStr">
-        <is>
-          <t>MOM</t>
-        </is>
-      </c>
-      <c r="B54">
-        <f>-1*SUMIF(J2:J45,"mom",H2:H45)</f>
-        <v/>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B48">
-    <cfRule type="cellIs" priority="1" operator="greaterThan" dxfId="14">
+  <conditionalFormatting sqref="B37">
+    <cfRule type="cellIs" priority="1" operator="greaterThan" dxfId="28">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="15">
+    <cfRule type="cellIs" priority="2" operator="lessThan" dxfId="29">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="cellIs" priority="3" operator="greaterThan" dxfId="14">
+  <conditionalFormatting sqref="B38">
+    <cfRule type="cellIs" priority="3" operator="greaterThan" dxfId="28">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="lessThan" dxfId="15">
+    <cfRule type="cellIs" priority="4" operator="lessThan" dxfId="29">
       <formula>80</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
-    <cfRule type="cellIs" priority="5" operator="greaterThan" dxfId="14">
+  <conditionalFormatting sqref="B39">
+    <cfRule type="cellIs" priority="5" operator="greaterThan" dxfId="28">
       <formula>300</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="6" operator="lessThan" dxfId="15">
+    <cfRule type="cellIs" priority="6" operator="lessThan" dxfId="29">
       <formula>300</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
-    <cfRule type="cellIs" priority="7" operator="greaterThan" dxfId="14">
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" priority="7" operator="greaterThan" dxfId="28">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="lessThan" dxfId="15">
+    <cfRule type="cellIs" priority="8" operator="lessThan" dxfId="29">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
-    <cfRule type="cellIs" priority="9" operator="greaterThan" dxfId="14">
+  <conditionalFormatting sqref="B41">
+    <cfRule type="cellIs" priority="9" operator="greaterThan" dxfId="28">
       <formula>300</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="lessThan" dxfId="15">
+    <cfRule type="cellIs" priority="10" operator="lessThan" dxfId="29">
       <formula>300</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B53">
-    <cfRule type="cellIs" priority="11" operator="greaterThan" dxfId="14">
+  <conditionalFormatting sqref="B42">
+    <cfRule type="cellIs" priority="11" operator="greaterThan" dxfId="28">
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="12" operator="lessThan" dxfId="15">
+    <cfRule type="cellIs" priority="12" operator="lessThan" dxfId="29">
       <formula>500</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
-    <cfRule type="cellIs" priority="13" operator="greaterThan" dxfId="14">
+  <conditionalFormatting sqref="B43">
+    <cfRule type="cellIs" priority="13" operator="greaterThan" dxfId="28">
       <formula>150</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="14" operator="lessThan" dxfId="15">
+    <cfRule type="cellIs" priority="14" operator="lessThan" dxfId="29">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added legend to end of excel, registered styles correctly
</commit_message>
<xml_diff>
--- a/output/BUDGETtest.xlsx
+++ b/output/BUDGETtest.xlsx
@@ -24,7 +24,7 @@
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
     <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <name val="Calibri"/>
       <color indexed="8"/>
@@ -98,8 +98,14 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <strike val="0"/>
+      <sz val="15"/>
+    </font>
+    <font/>
   </fonts>
-  <fills count="13">
+  <fills count="17">
     <fill>
       <patternFill/>
     </fill>
@@ -171,8 +177,31 @@
         <fgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF9900"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EE1111"/>
+        <bgColor rgb="00EE1111"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000CCFF"/>
+        <bgColor rgb="0000CCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -493,13 +522,36 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="25" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="25" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="26"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="26"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -596,11 +648,28 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="20" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="5">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="26" pivotButton="0" quotePrefix="0" xfId="5"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="5">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="26" pivotButton="0" quotePrefix="0" xfId="5"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="5">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
-    <cellStyle name="header" xfId="2"/>
+    <cellStyle name="template" xfId="5" hidden="0"/>
+    <cellStyle name="header" xfId="5" hidden="0"/>
+    <cellStyle name="redFill" xfId="5" hidden="0"/>
+    <cellStyle name="blueFill" xfId="5" hidden="0"/>
   </cellStyles>
   <dxfs count="30">
     <dxf>
@@ -5516,13 +5585,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="11.07" customWidth="1" min="1" max="1"/>
     <col width="44.28" customWidth="1" min="2" max="2"/>
@@ -7034,7 +7103,7 @@
     <row r="46"/>
     <row r="47"/>
     <row r="48">
-      <c r="A48" s="42" t="inlineStr">
+      <c r="A48" s="49" t="inlineStr">
         <is>
           <t>TRANSPORT</t>
         </is>
@@ -7045,7 +7114,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="42" t="inlineStr">
+      <c r="A49" s="49" t="inlineStr">
         <is>
           <t>PHONE</t>
         </is>
@@ -7056,7 +7125,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="42" t="inlineStr">
+      <c r="A50" s="49" t="inlineStr">
         <is>
           <t>SHOPPING</t>
         </is>
@@ -7067,7 +7136,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="42" t="inlineStr">
+      <c r="A51" s="49" t="inlineStr">
         <is>
           <t>ACTIVITY</t>
         </is>
@@ -7078,7 +7147,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="42" t="inlineStr">
+      <c r="A52" s="49" t="inlineStr">
         <is>
           <t>FOOD</t>
         </is>
@@ -7089,7 +7158,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="42" t="inlineStr">
+      <c r="A53" s="49" t="inlineStr">
         <is>
           <t>GROCERY</t>
         </is>
@@ -7100,7 +7169,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="42" t="inlineStr">
+      <c r="A54" s="49" t="inlineStr">
         <is>
           <t>MOM</t>
         </is>
@@ -7108,6 +7177,20 @@
       <c r="B54">
         <f>-1*SUMIF(J2:J45,"mom",H2:H45)</f>
         <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" s="46" t="inlineStr">
+        <is>
+          <t>OVERSPENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" s="48" t="inlineStr">
+        <is>
+          <t>UNDERSPENT</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>